<commit_message>
feat: added parser for formulas
</commit_message>
<xml_diff>
--- a/test/master-detail.xlsx
+++ b/test/master-detail.xlsx
@@ -159,11 +159,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Verdana"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -203,13 +203,8 @@
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Verdana"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FF1F2328"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -304,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -368,11 +363,17 @@
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
@@ -380,28 +381,31 @@
     <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
     <xf borderId="2" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -425,52 +429,52 @@
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:srgbClr val="1A2F40"/>
       </a:dk1>
       <a:lt1>
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="000000"/>
+        <a:srgbClr val="1A2F40"/>
       </a:dk2>
       <a:lt2>
         <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="C93232"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="E27228"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="0D398C"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="FC4479"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="DCDC12"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="1F95D1"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="1F95D1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="1F95D1"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Verdana"/>
+        <a:ea typeface="Verdana"/>
+        <a:cs typeface="Verdana"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Verdana"/>
+        <a:ea typeface="Verdana"/>
+        <a:cs typeface="Verdana"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -622,15 +626,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="36.63"/>
-    <col customWidth="1" min="2" max="2" width="26.5"/>
-    <col customWidth="1" min="3" max="3" width="34.63"/>
-    <col customWidth="1" min="4" max="4" width="40.38"/>
-    <col customWidth="1" min="5" max="5" width="37.25"/>
-    <col customWidth="1" min="6" max="6" width="28.0"/>
-    <col customWidth="1" min="7" max="7" width="29.63"/>
+    <col customWidth="1" min="1" max="1" width="32.56"/>
+    <col customWidth="1" min="2" max="2" width="23.56"/>
+    <col customWidth="1" min="3" max="3" width="30.78"/>
+    <col customWidth="1" min="4" max="4" width="35.89"/>
+    <col customWidth="1" min="5" max="5" width="33.11"/>
+    <col customWidth="1" min="6" max="6" width="24.89"/>
+    <col customWidth="1" min="7" max="7" width="26.33"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -840,20 +844,20 @@
       <c r="B17" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="21" t="str">
+      <c r="E17" s="22" t="str">
         <f>D17-C17</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="23">
         <v>10.0</v>
       </c>
-      <c r="G17" s="22" t="str">
+      <c r="G17" s="23" t="str">
         <f>E17*F17*24</f>
         <v>#VALUE!</v>
       </c>
@@ -861,29 +865,29 @@
     </row>
     <row r="18">
       <c r="A18" s="18"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
       <c r="H18" s="4"/>
     </row>
     <row r="19">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25" t="s">
+      <c r="A19" s="26"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="26" t="str">
+      <c r="E19" s="29" t="str">
         <f>SUM(E16:E18)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="28" t="str">
+      <c r="G19" s="31" t="str">
         <f>SUM(G16:G18)</f>
         <v>#VALUE!</v>
       </c>
@@ -902,17 +906,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.25"/>
-    <col customWidth="1" min="2" max="2" width="20.13"/>
-    <col customWidth="1" min="3" max="3" width="15.5"/>
-    <col customWidth="1" min="4" max="4" width="13.5"/>
-    <col customWidth="1" min="5" max="5" width="16.38"/>
+    <col customWidth="1" min="1" max="1" width="19.78"/>
+    <col customWidth="1" min="2" max="2" width="17.89"/>
+    <col customWidth="1" min="3" max="3" width="13.78"/>
+    <col customWidth="1" min="4" max="4" width="12.0"/>
+    <col customWidth="1" min="5" max="5" width="14.56"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="4"/>
@@ -921,7 +925,7 @@
       <c r="E1" s="4"/>
     </row>
     <row r="2">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="33" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="4"/>
@@ -930,7 +934,7 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="32" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="4"/>
@@ -939,7 +943,7 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="32" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="4"/>
@@ -948,7 +952,7 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="32" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="4"/>
@@ -978,7 +982,7 @@
       <c r="E8" s="4"/>
     </row>
     <row r="9">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="32" t="s">
         <v>34</v>
       </c>
       <c r="B9" s="4"/>
@@ -987,36 +991,36 @@
       <c r="E9" s="4"/>
     </row>
     <row r="10">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="34" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="32" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1042,7 +1046,7 @@
       <c r="E14" s="4"/>
     </row>
     <row r="15">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="32" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="4"/>
@@ -1051,39 +1055,39 @@
       <c r="E15" s="4"/>
     </row>
     <row r="16">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="34" t="s">
         <v>37</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
     <row r="17">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="32" t="s">
         <v>32</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
     <row r="18">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="32" t="s">
         <v>32</v>
       </c>
       <c r="D18" s="4"/>

</xml_diff>